<commit_message>
Importa as quotes R
</commit_message>
<xml_diff>
--- a/Lista IBrX50.xlsx
+++ b/Lista IBrX50.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="122">
   <si>
     <t>Ação</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>Não (IPO 2017)</t>
+  </si>
+  <si>
+    <t>Não (Entender)</t>
   </si>
 </sst>
 </file>
@@ -826,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,23 +1704,23 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D44" s="2">
+      <c r="C44" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="13">
         <v>751848759</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="14">
         <v>1.6040000000000001</v>
       </c>
-      <c r="F44" s="15" t="s">
-        <v>118</v>
+      <c r="F44" s="16" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implementa o grafico - long
</commit_message>
<xml_diff>
--- a/Lista IBrX50.xlsx
+++ b/Lista IBrX50.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Controle" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="124">
   <si>
     <t>Ação</t>
   </si>
@@ -380,10 +380,13 @@
     <t>Não (IPO 2017)</t>
   </si>
   <si>
-    <t>Não (Entender)</t>
-  </si>
-  <si>
-    <t>Não deixa rodar</t>
+    <t>Cotação tudo errada</t>
+  </si>
+  <si>
+    <t>Não deixa rodar, existem linhas NULL na cotação, rever</t>
+  </si>
+  <si>
+    <t>Não (Arrumar)</t>
   </si>
 </sst>
 </file>
@@ -393,8 +396,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0000%"/>
-    <numFmt numFmtId="175" formatCode="0.00000000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="0.00000000%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -427,7 +430,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,12 +446,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,7 +492,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -537,20 +534,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,23 +1677,23 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D42" s="18">
+      <c r="D42" s="13">
         <v>372112887</v>
       </c>
-      <c r="E42" s="19">
+      <c r="E42" s="14">
         <v>1.073</v>
       </c>
-      <c r="F42" s="20" t="s">
-        <v>118</v>
+      <c r="F42" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="G42" t="s">
         <v>122</v>
@@ -1751,6 +1736,9 @@
         <v>1.6040000000000001</v>
       </c>
       <c r="F44" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="G44" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1930,27 +1918,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="21"/>
+    <col min="2" max="2" width="12.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="22">
+      <c r="B1" s="18">
         <v>1.0205402970314E-2</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="21">
+      <c r="N1" s="17">
         <v>1.1006981134414701E-2</v>
       </c>
     </row>
@@ -1958,13 +1946,13 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="18">
         <v>1.6997143626213101E-2</v>
       </c>
       <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="21">
+      <c r="N2" s="17">
         <v>2.1389320492744401E-2</v>
       </c>
     </row>
@@ -1972,13 +1960,13 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="18">
         <v>9.6000432968139596E-3</v>
       </c>
       <c r="M3" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="21">
+      <c r="N3" s="17">
         <v>1.03187710046768E-2</v>
       </c>
     </row>
@@ -1986,13 +1974,13 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="18">
         <v>2.0845681428909298E-2</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="17">
         <v>2.87328511476517E-2</v>
       </c>
     </row>
@@ -2000,13 +1988,13 @@
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="18">
         <v>1.53200030326843E-2</v>
       </c>
       <c r="M5" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="21">
+      <c r="N5" s="17">
         <v>1.5738204121589699E-2</v>
       </c>
     </row>
@@ -2014,13 +2002,13 @@
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="18">
         <v>1.2514993548393199E-2</v>
       </c>
       <c r="M6" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="21">
+      <c r="N6" s="17">
         <v>1.2296915054321299E-2</v>
       </c>
     </row>
@@ -2028,13 +2016,13 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="18">
         <v>5.3032338619232199E-2</v>
       </c>
       <c r="M7" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="21">
+      <c r="N7" s="17">
         <v>5.8149978518486002E-2</v>
       </c>
     </row>
@@ -2042,13 +2030,13 @@
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="18">
         <v>2.7540028095245399E-2</v>
       </c>
       <c r="M8" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="17">
         <v>1.10453367233276E-2</v>
       </c>
     </row>
@@ -2056,13 +2044,13 @@
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="18">
         <v>3.00468355417252E-2</v>
       </c>
       <c r="M9" t="s">
         <v>27</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="17">
         <v>3.1246110796928399E-2</v>
       </c>
     </row>
@@ -2070,13 +2058,13 @@
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="18">
         <v>4.2544856667518602E-2</v>
       </c>
       <c r="M10" t="s">
         <v>30</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="17">
         <v>2.7405500411987301E-2</v>
       </c>
     </row>
@@ -2084,13 +2072,13 @@
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="18">
         <v>1.9897431135177598E-2</v>
       </c>
       <c r="M11" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="17">
         <v>2.15539634227753E-2</v>
       </c>
     </row>
@@ -2098,13 +2086,13 @@
       <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="18">
         <v>2.9746145009994498E-3</v>
       </c>
       <c r="M12" t="s">
         <v>34</v>
       </c>
-      <c r="N12" s="21">
+      <c r="N12" s="17">
         <v>3.8679391145706198E-3</v>
       </c>
     </row>
@@ -2112,13 +2100,13 @@
       <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="18">
         <v>7.0401281118392901E-3</v>
       </c>
       <c r="M13" t="s">
         <v>36</v>
       </c>
-      <c r="N13" s="21">
+      <c r="N13" s="17">
         <v>7.4044167995452898E-3</v>
       </c>
     </row>
@@ -2126,13 +2114,13 @@
       <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="18">
         <v>1.85133963823318E-2</v>
       </c>
       <c r="M14" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="21">
+      <c r="N14" s="17">
         <v>1.9843727350234999E-2</v>
       </c>
     </row>
@@ -2140,13 +2128,13 @@
       <c r="A15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="18">
         <v>1.8495753407478301E-2</v>
       </c>
       <c r="M15" t="s">
         <v>41</v>
       </c>
-      <c r="N15" s="21">
+      <c r="N15" s="17">
         <v>2.00339704751968E-2</v>
       </c>
     </row>
@@ -2154,13 +2142,13 @@
       <c r="A16" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="18">
         <v>1.9463196396827701E-2</v>
       </c>
       <c r="M16" t="s">
         <v>43</v>
       </c>
-      <c r="N16" s="21">
+      <c r="N16" s="17">
         <v>2.2428184747695899E-2</v>
       </c>
     </row>
@@ -2168,13 +2156,13 @@
       <c r="A17" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="18">
         <v>5.2720725536346401E-2</v>
       </c>
       <c r="M17" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="21">
+      <c r="N17" s="17">
         <v>5.3984552621841403E-2</v>
       </c>
     </row>
@@ -2182,13 +2170,13 @@
       <c r="A18" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="18">
         <v>1.1198312044143699E-2</v>
       </c>
       <c r="M18" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="21">
+      <c r="N18" s="17">
         <v>1.6776412725448601E-2</v>
       </c>
     </row>
@@ -2196,13 +2184,13 @@
       <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="18">
         <v>1.6872957348823499E-2</v>
       </c>
       <c r="M19" t="s">
         <v>49</v>
       </c>
-      <c r="N19" s="21">
+      <c r="N19" s="17">
         <v>1.7462015151977501E-2</v>
       </c>
     </row>
@@ -2210,13 +2198,13 @@
       <c r="A20" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="18">
         <v>2.7487441897392301E-2</v>
       </c>
       <c r="M20" t="s">
         <v>51</v>
       </c>
-      <c r="N20" s="21">
+      <c r="N20" s="17">
         <v>2.9045596718788098E-2</v>
       </c>
     </row>
@@ -2224,13 +2212,13 @@
       <c r="A21" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="18">
         <v>1.7522215843200701E-2</v>
       </c>
       <c r="M21" t="s">
         <v>53</v>
       </c>
-      <c r="N21" s="21">
+      <c r="N21" s="17">
         <v>1.7835617065429701E-2</v>
       </c>
     </row>
@@ -2238,13 +2226,13 @@
       <c r="A22" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="18">
         <v>3.02833765745163E-2</v>
       </c>
       <c r="M22" t="s">
         <v>55</v>
       </c>
-      <c r="N22" s="21">
+      <c r="N22" s="17">
         <v>1.8097981810569801E-2</v>
       </c>
     </row>
@@ -2252,13 +2240,13 @@
       <c r="A23" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="18">
         <v>1.9537553191185001E-2</v>
       </c>
       <c r="M23" t="s">
         <v>57</v>
       </c>
-      <c r="N23" s="21">
+      <c r="N23" s="17">
         <v>2.3380979895591701E-2</v>
       </c>
     </row>
@@ -2266,13 +2254,13 @@
       <c r="A24" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="18">
         <v>1.31618082523346E-2</v>
       </c>
       <c r="M24" t="s">
         <v>60</v>
       </c>
-      <c r="N24" s="21">
+      <c r="N24" s="17">
         <v>1.4684632420539899E-2</v>
       </c>
     </row>
@@ -2280,13 +2268,13 @@
       <c r="A25" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="18">
         <v>3.4456372261047398E-2</v>
       </c>
       <c r="M25" t="s">
         <v>62</v>
       </c>
-      <c r="N25" s="21">
+      <c r="N25" s="17">
         <v>8.8009685277938808E-3</v>
       </c>
     </row>
@@ -2294,13 +2282,13 @@
       <c r="A26" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="18">
         <v>3.3468514680862399E-2</v>
       </c>
       <c r="M26" t="s">
         <v>64</v>
       </c>
-      <c r="N26" s="21">
+      <c r="N26" s="17">
         <v>3.5149976611137397E-2</v>
       </c>
     </row>
@@ -2308,13 +2296,13 @@
       <c r="A27" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="18">
         <v>2.2154092788696299E-2</v>
       </c>
       <c r="M27" t="s">
         <v>69</v>
       </c>
-      <c r="N27" s="21">
+      <c r="N27" s="17">
         <v>2.4416044354438799E-2</v>
       </c>
     </row>
@@ -2322,13 +2310,13 @@
       <c r="A28" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B28" s="18">
         <v>2.4127081036567698E-2</v>
       </c>
       <c r="M28" t="s">
         <v>71</v>
       </c>
-      <c r="N28" s="21">
+      <c r="N28" s="17">
         <v>3.10169160366058E-3</v>
       </c>
     </row>
@@ -2336,13 +2324,13 @@
       <c r="A29" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="22">
+      <c r="B29" s="18">
         <v>6.9707036018371599E-3</v>
       </c>
       <c r="M29" t="s">
         <v>73</v>
       </c>
-      <c r="N29" s="21">
+      <c r="N29" s="17">
         <v>1.5369728207588199E-2</v>
       </c>
     </row>
@@ -2350,13 +2338,13 @@
       <c r="A30" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="18">
         <v>4.49936091899872E-3</v>
       </c>
       <c r="M30" t="s">
         <v>75</v>
       </c>
-      <c r="N30" s="21">
+      <c r="N30" s="17">
         <v>7.4144452810287502E-3</v>
       </c>
     </row>
@@ -2364,13 +2352,13 @@
       <c r="A31" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="22">
+      <c r="B31" s="18">
         <v>2.7629956603050201E-2</v>
       </c>
       <c r="M31" t="s">
         <v>77</v>
       </c>
-      <c r="N31" s="21">
+      <c r="N31" s="17">
         <v>3.11166048049927E-2</v>
       </c>
     </row>
@@ -2378,13 +2366,13 @@
       <c r="A32" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="22">
+      <c r="B32" s="18">
         <v>2.4226993322372398E-2</v>
       </c>
       <c r="M32" t="s">
         <v>80</v>
       </c>
-      <c r="N32" s="21">
+      <c r="N32" s="17">
         <v>2.8706848621368401E-2</v>
       </c>
     </row>
@@ -2392,13 +2380,13 @@
       <c r="A33" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="18">
         <v>9.0640634298324602E-3</v>
       </c>
       <c r="M33" t="s">
         <v>82</v>
       </c>
-      <c r="N33" s="21">
+      <c r="N33" s="17">
         <v>1.3297826051712E-2</v>
       </c>
     </row>
@@ -2406,13 +2394,13 @@
       <c r="A34" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="22">
+      <c r="B34" s="18">
         <v>2.2082656621933001E-2</v>
       </c>
       <c r="M34" t="s">
         <v>84</v>
       </c>
-      <c r="N34" s="21">
+      <c r="N34" s="17">
         <v>1.25094801187515E-2</v>
       </c>
     </row>
@@ -2420,7 +2408,7 @@
       <c r="A35" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="22">
+      <c r="B35" s="18">
         <v>1.9783154129982002E-2</v>
       </c>
       <c r="I35">
@@ -2429,7 +2417,7 @@
       <c r="M35" t="s">
         <v>86</v>
       </c>
-      <c r="N35" s="21">
+      <c r="N35" s="17">
         <v>2.1028488874435401E-2</v>
       </c>
     </row>
@@ -2437,7 +2425,7 @@
       <c r="A36" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="22">
+      <c r="B36" s="18">
         <v>1.8988057971000699E-2</v>
       </c>
       <c r="I36">
@@ -2447,7 +2435,7 @@
       <c r="M36" t="s">
         <v>87</v>
       </c>
-      <c r="N36" s="21">
+      <c r="N36" s="17">
         <v>1.99665725231171E-2</v>
       </c>
     </row>
@@ -2455,13 +2443,13 @@
       <c r="A37" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="22">
+      <c r="B37" s="18">
         <v>2.7664005756378202E-2</v>
       </c>
       <c r="M37" t="s">
         <v>89</v>
       </c>
-      <c r="N37" s="21">
+      <c r="N37" s="17">
         <v>2.4331405758857699E-2</v>
       </c>
     </row>
@@ -2469,13 +2457,13 @@
       <c r="A38" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="22">
+      <c r="B38" s="18">
         <v>2.7082473039627099E-2</v>
       </c>
       <c r="M38" t="s">
         <v>91</v>
       </c>
-      <c r="N38" s="21">
+      <c r="N38" s="17">
         <v>3.2349199056625401E-2</v>
       </c>
     </row>
@@ -2483,13 +2471,13 @@
       <c r="A39" t="s">
         <v>96</v>
       </c>
-      <c r="B39" s="22">
+      <c r="B39" s="18">
         <v>2.6804685592651398E-2</v>
       </c>
       <c r="M39" t="s">
         <v>96</v>
       </c>
-      <c r="N39" s="21">
+      <c r="N39" s="17">
         <v>3.0283838510513299E-2</v>
       </c>
     </row>
@@ -2497,13 +2485,13 @@
       <c r="A40" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="22">
+      <c r="B40" s="18">
         <v>2.27248966693878E-2</v>
       </c>
       <c r="M40" t="s">
         <v>100</v>
       </c>
-      <c r="N40" s="21">
+      <c r="N40" s="17">
         <v>2.4108424782753001E-2</v>
       </c>
     </row>
@@ -2511,13 +2499,13 @@
       <c r="A41" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="22">
+      <c r="B41" s="18">
         <v>2.9783174395561201E-2</v>
       </c>
       <c r="M41" t="s">
         <v>102</v>
       </c>
-      <c r="N41" s="21">
+      <c r="N41" s="17">
         <v>3.2681182026863098E-2</v>
       </c>
     </row>
@@ -2525,13 +2513,13 @@
       <c r="A42" t="s">
         <v>104</v>
       </c>
-      <c r="B42" s="22">
+      <c r="B42" s="18">
         <v>2.4296715855598401E-2</v>
       </c>
       <c r="M42" t="s">
         <v>104</v>
       </c>
-      <c r="N42" s="21">
+      <c r="N42" s="17">
         <v>2.62444317340851E-2</v>
       </c>
     </row>
@@ -2539,13 +2527,13 @@
       <c r="A43" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="22">
+      <c r="B43" s="18">
         <v>2.3487105965614302E-2</v>
       </c>
       <c r="M43" t="s">
         <v>106</v>
       </c>
-      <c r="N43" s="21">
+      <c r="N43" s="17">
         <v>2.5662213563919099E-2</v>
       </c>
     </row>
@@ -2553,13 +2541,13 @@
       <c r="A44" t="s">
         <v>108</v>
       </c>
-      <c r="B44" s="22">
+      <c r="B44" s="18">
         <v>3.1843170523643501E-2</v>
       </c>
       <c r="M44" t="s">
         <v>108</v>
       </c>
-      <c r="N44" s="21">
+      <c r="N44" s="17">
         <v>3.4460917115211501E-2</v>
       </c>
     </row>
@@ -2567,13 +2555,13 @@
       <c r="A45" t="s">
         <v>111</v>
       </c>
-      <c r="B45" s="22">
+      <c r="B45" s="18">
         <v>4.7760754823684701E-3</v>
       </c>
       <c r="M45" t="s">
         <v>111</v>
       </c>
-      <c r="N45" s="21">
+      <c r="N45" s="17">
         <v>5.4378509521484401E-3</v>
       </c>
     </row>
@@ -2581,13 +2569,13 @@
       <c r="A46" t="s">
         <v>113</v>
       </c>
-      <c r="B46" s="22">
+      <c r="B46" s="18">
         <v>2.54222452640533E-2</v>
       </c>
       <c r="M46" t="s">
         <v>113</v>
       </c>
-      <c r="N46" s="21">
+      <c r="N46" s="17">
         <v>2.9856905341148401E-2</v>
       </c>
     </row>

</xml_diff>